<commit_message>
Add corp info to docs
</commit_message>
<xml_diff>
--- a/storage/app/exel_templates/market_check.xlsx
+++ b/storage/app/exel_templates/market_check.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>Товарный чек №</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>Продавец</t>
-  </si>
-  <si>
-    <t>ООО Эргон</t>
   </si>
   <si>
     <t>Имя</t>
@@ -43,10 +40,6 @@
   </si>
   <si>
     <t>Адрес</t>
-  </si>
-  <si>
-    <t>117041, г.Москва, ул.Адмирала 
-Лазарева, д.42, эт.1 пом.VII, ком.4</t>
   </si>
   <si>
     <t>Время</t>
@@ -176,11 +169,23 @@
   <si>
     <t>от %date%</t>
   </si>
+  <si>
+    <t>%corporate_name%</t>
+  </si>
+  <si>
+    <t>%corporate_inn%</t>
+  </si>
+  <si>
+    <t>%corporate_ogrn%</t>
+  </si>
+  <si>
+    <t>%corporate_address%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,6 +458,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -500,7 +508,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,7 +543,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -747,7 +755,7 @@
   <dimension ref="A1:R995"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="80" zoomScaleNormal="60" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,10 +775,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
@@ -790,13 +798,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="E3" s="27"/>
       <c r="F3" s="27"/>
@@ -804,16 +812,16 @@
     </row>
     <row r="4" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="28">
-        <v>1187746512700</v>
+      <c r="D4" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
@@ -821,16 +829,16 @@
     </row>
     <row r="5" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="28">
-        <v>7727354975</v>
+      <c r="D5" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="E5" s="28"/>
       <c r="F5" s="28"/>
@@ -838,16 +846,16 @@
     </row>
     <row r="6" spans="1:18" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
@@ -855,16 +863,16 @@
     </row>
     <row r="7" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -881,51 +889,51 @@
     </row>
     <row r="9" spans="1:18" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="10" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="G10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="12" t="s">
+      <c r="R10" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="R10" s="12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -939,7 +947,7 @@
     </row>
     <row r="12" spans="1:18" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="24"/>
@@ -959,7 +967,7 @@
     </row>
     <row r="14" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -979,13 +987,13 @@
     </row>
     <row r="16" spans="1:18" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="3"/>
@@ -995,10 +1003,10 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1012,7 +1020,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G18" s="4"/>
     </row>

</xml_diff>